<commit_message>
Changes made for Telemundo runs
</commit_message>
<xml_diff>
--- a/MasterData/10. AmortTemplateE!.xlsx
+++ b/MasterData/10. AmortTemplateE!.xlsx
@@ -216,12 +216,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -236,10 +242,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +531,7 @@
   <dimension ref="A1:F192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E139" sqref="E139:E143"/>
+      <selection activeCell="F144" sqref="F144:F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3397,7 +3404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>150</v>
       </c>
@@ -3417,7 +3424,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>150</v>
       </c>
@@ -3437,7 +3444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>150</v>
       </c>
@@ -3457,7 +3464,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>150</v>
       </c>
@@ -3477,7 +3484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>150</v>
       </c>
@@ -4382,11 +4389,6 @@
     <filterColumn colId="0">
       <filters>
         <filter val="150"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Bio/Clip (E)"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4404,7 +4406,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:A37"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6062,13 +6064,13 @@
       <c r="A37" s="1">
         <v>150</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E37" s="1" t="s">

</xml_diff>

<commit_message>
Oxygen and E! results updated
</commit_message>
<xml_diff>
--- a/MasterData/10. AmortTemplateE!.xlsx
+++ b/MasterData/10. AmortTemplateE!.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AmortTemplateSectionGrid" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="55">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
@@ -4388,12 +4388,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4460,7 +4457,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>136</v>
       </c>
@@ -4505,7 +4502,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>136</v>
       </c>
@@ -4550,7 +4547,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>136</v>
       </c>
@@ -4595,7 +4592,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>136</v>
       </c>
@@ -4640,7 +4637,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>136</v>
       </c>
@@ -4685,7 +4682,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>136</v>
       </c>
@@ -4730,7 +4727,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>136</v>
       </c>
@@ -4775,7 +4772,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>137</v>
       </c>
@@ -4820,7 +4817,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>137</v>
       </c>
@@ -4865,7 +4862,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>137</v>
       </c>
@@ -4910,7 +4907,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>137</v>
       </c>
@@ -4955,7 +4952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>137</v>
       </c>
@@ -5003,7 +5000,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>137</v>
       </c>
@@ -5048,7 +5045,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>137</v>
       </c>
@@ -5093,7 +5090,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>137</v>
       </c>
@@ -5138,7 +5135,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>137</v>
       </c>
@@ -5183,7 +5180,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>137</v>
       </c>
@@ -5228,7 +5225,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>137</v>
       </c>
@@ -5273,7 +5270,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>138</v>
       </c>
@@ -5318,7 +5315,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>138</v>
       </c>
@@ -5363,7 +5360,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>138</v>
       </c>
@@ -5408,7 +5405,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>138</v>
       </c>
@@ -5453,7 +5450,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>138</v>
       </c>
@@ -5498,7 +5495,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>138</v>
       </c>
@@ -5543,7 +5540,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>138</v>
       </c>
@@ -5588,7 +5585,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>146</v>
       </c>
@@ -5633,7 +5630,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>146</v>
       </c>
@@ -5678,7 +5675,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>147</v>
       </c>
@@ -5723,7 +5720,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>147</v>
       </c>
@@ -5768,7 +5765,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>148</v>
       </c>
@@ -5813,7 +5810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>148</v>
       </c>
@@ -5858,7 +5855,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>148</v>
       </c>
@@ -5903,7 +5900,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>149</v>
       </c>
@@ -5948,7 +5945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>149</v>
       </c>
@@ -6034,9 +6031,8 @@
         <f t="shared" si="0"/>
         <v>150THSBio/Clip (E)Bio/Clip (E)</v>
       </c>
-      <c r="N36" s="1" t="e">
-        <f>VLOOKUP(M36,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
+      <c r="N36" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -6080,12 +6076,11 @@
         <f t="shared" si="0"/>
         <v>150THSOriginal SeriesBio/Clip (E)</v>
       </c>
-      <c r="N37" s="1" t="e">
-        <f>VLOOKUP(M37,Results!F:F,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N37" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>169</v>
       </c>
@@ -6133,7 +6128,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>169</v>
       </c>
@@ -6181,7 +6176,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>169</v>
       </c>
@@ -6229,7 +6224,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>169</v>
       </c>
@@ -6277,7 +6272,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>169</v>
       </c>
@@ -6325,7 +6320,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>169</v>
       </c>
@@ -6373,7 +6368,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>169</v>
       </c>
@@ -6421,7 +6416,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>169</v>
       </c>
@@ -6469,7 +6464,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>169</v>
       </c>
@@ -6517,7 +6512,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>169</v>
       </c>
@@ -6565,7 +6560,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>169</v>
       </c>
@@ -6613,7 +6608,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>172</v>
       </c>
@@ -6661,7 +6656,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>172</v>
       </c>
@@ -6709,7 +6704,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>172</v>
       </c>
@@ -6757,7 +6752,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>172</v>
       </c>
@@ -6805,7 +6800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>368</v>
       </c>
@@ -6853,7 +6848,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>368</v>
       </c>
@@ -6901,7 +6896,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>368</v>
       </c>
@@ -6949,7 +6944,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>368</v>
       </c>
@@ -6998,13 +6993,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O56">
-    <filterColumn colId="13">
-      <filters>
-        <filter val="#N/A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -7018,7 +7006,7 @@
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:E34"/>
+      <selection activeCell="A35" sqref="A35:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7740,15 +7728,45 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>150</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" t="s">
+        <v>52</v>
+      </c>
       <c r="F35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>150THSBio/Clip (E)Bio/Clip (E)</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>150</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
+        <v>52</v>
+      </c>
       <c r="F36" s="1" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>150THSOriginal SeriesBio/Clip (E)</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>